<commit_message>
update one pager and remove redundant README text from the template itself
</commit_message>
<xml_diff>
--- a/template/accdcTemplateOutsideSubmission.xlsx
+++ b/template/accdcTemplateOutsideSubmission.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\outsideSubmissionTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\outsideSubmissionTemplate\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE00C4D-9D98-4828-B723-4CC6E638F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A102C5-69C9-4B5F-B394-A800A48C4E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13005" yWindow="1080" windowWidth="15795" windowHeight="15120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="885" windowWidth="28335" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_v0-00" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>REFNUM</t>
   </si>
@@ -265,16 +265,13 @@
     <t>OBTIMEend</t>
   </si>
   <si>
-    <t>to find metadata associated with this template ("data dictionary"), go to our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate</t>
-  </si>
-  <si>
-    <t>to make sure you have to most up-to-date version, download this file directly from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate</t>
-  </si>
-  <si>
-    <t>to provide feedback on this template, please submit this Google form</t>
-  </si>
-  <si>
-    <t>or create an issue on the issue tracker</t>
+    <t>IMPORTANT</t>
+  </si>
+  <si>
+    <t>Read this doc first: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate/blob/main/docs/accdcHowToSubmitData.pdf</t>
+  </si>
+  <si>
+    <t>To make sure you have to most up-to-date version, download the template directly from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate</t>
   </si>
 </sst>
 </file>
@@ -285,7 +282,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +345,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -377,7 +382,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -419,6 +424,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1089,43 +1096,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0B503C-45C2-4682-A279-7D9876A20A9B}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>75</v>
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>77</v>
-      </c>
+      <c r="A4" s="14"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="to make sure you have to most up to date version, download this file from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{68273A7E-5932-4AB3-916D-F05551D05E2C}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{FA7FC906-4AAA-411C-83EE-13BA40AD1AF7}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{4045D2E4-E1DA-4C81-BF39-5ED34065FEC4}"/>
+    <hyperlink ref="A3" r:id="rId1" display="to make sure you have to most up to date version, download this file from our repo: https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{6915430C-55DD-436F-A74B-E2345D056ECD}"/>
+    <hyperlink ref="A2" r:id="rId2" display="Read this doc first" xr:uid="{6A905369-B841-4FFA-AD4F-39C517722E0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
remove dropdowns on OBABUN, OBEVID, OBABUNSITE and PROTOCOL
</commit_message>
<xml_diff>
--- a/template/accdcTemplateOutsideSubmission.xlsx
+++ b/template/accdcTemplateOutsideSubmission.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\01 - PROJECTS\537_observationTemplate\outsideSubmissionTemplate\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A102C5-69C9-4B5F-B394-A800A48C4E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583ADAC9-F44B-46DC-94AB-B3E558C67CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="885" windowWidth="28335" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="990" windowWidth="17310" windowHeight="13410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_v0-00" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="6" r:id="rId2"/>
-    <sheet name="OBEVID" sheetId="2" r:id="rId3"/>
-    <sheet name="OBABUN" sheetId="3" r:id="rId4"/>
-    <sheet name="OBABUNSITE" sheetId="4" r:id="rId5"/>
-    <sheet name="PROTOCOL" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'template_v0-00'!$A$1:$AX$2</definedName>
@@ -41,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>REFNUM</t>
   </si>
@@ -185,78 +181,6 @@
   </si>
   <si>
     <t>obDATEverbatim</t>
-  </si>
-  <si>
-    <t>specimen</t>
-  </si>
-  <si>
-    <t>photo</t>
-  </si>
-  <si>
-    <t>specimen;photo</t>
-  </si>
-  <si>
-    <t>aural detection</t>
-  </si>
-  <si>
-    <t>sound recording</t>
-  </si>
-  <si>
-    <t>video recording</t>
-  </si>
-  <si>
-    <t>indirect (e.g., scat, pellets, tracks, browse)</t>
-  </si>
-  <si>
-    <t>perennial nest site</t>
-  </si>
-  <si>
-    <t>iNaturalist</t>
-  </si>
-  <si>
-    <t>sight record</t>
-  </si>
-  <si>
-    <t>abundant</t>
-  </si>
-  <si>
-    <t>locally common</t>
-  </si>
-  <si>
-    <t>scattered</t>
-  </si>
-  <si>
-    <t>rare</t>
-  </si>
-  <si>
-    <t>common within survey site</t>
-  </si>
-  <si>
-    <t>rare within survey site</t>
-  </si>
-  <si>
-    <t>uncommon within survey site</t>
-  </si>
-  <si>
-    <t>incidental</t>
-  </si>
-  <si>
-    <t>point count</t>
-  </si>
-  <si>
-    <t>area search</t>
-  </si>
-  <si>
-    <t>trapping</t>
-  </si>
-  <si>
-    <t>songmeter</t>
-  </si>
-  <si>
-    <t>eBird - Travelling</t>
-  </si>
-  <si>
-    <t>eBird - Incidental</t>
   </si>
   <si>
     <t>OBTIME</t>
@@ -744,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -824,10 +748,10 @@
         <v>47</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>45</v>
@@ -1061,36 +985,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the OBEVID field. See the OBEVID tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{58890871-BB0B-4187-B053-BECAE26D70C2}">
-          <x14:formula1>
-            <xm:f>OBEVID!$A$1:$A$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>AD1:AD1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the OBABUN field. See the OBABUN tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{535D8599-9410-414A-8279-5DBB317BAB6C}">
-          <x14:formula1>
-            <xm:f>OBABUN!$A$1:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>AE1:AE1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the OBABUNSITE field. See the OBABUNSITE tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{281AA0A5-0C44-4F74-9371-6C6F2D49754A}">
-          <x14:formula1>
-            <xm:f>OBABUNSITE!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>AF1:AF1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="This value is not allowed in the PROTOCOL field. See the PROTOCOL tab for allowable values._x000a__x000a_See the README at https://github.com/atlanticcanadacdc/outsideSubmissionTemplate" xr:uid="{2DBE70EF-0781-49B6-9F67-E70BF08A9C65}">
-          <x14:formula1>
-            <xm:f>PROTOCOL!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>AR1:AR1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1106,17 +1000,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -1136,185 +1030,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB774BC8-9194-4144-975B-CFE4E7E3F552}">
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3900AA5-948C-4FE1-9D24-5854C30EABD8}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED745171-8CAD-48CA-A70F-98F1CC85585B}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7DD475-3512-455B-8B60-40854C146542}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>